<commit_message>
added DERS and fixed some things
</commit_message>
<xml_diff>
--- a/BUS 2.xlsx
+++ b/BUS 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4264522ea65d2ce8/Dokumenter/NTNU/Master/Python Code/Git Repo/Simple-System-for-Power-System-Reliability-Calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1011" documentId="11_AD4D1D646341095ACB70008C251E688C5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{649FB758-8A47-4EE9-9FAD-2681B39A81EF}"/>
+  <xr:revisionPtr revIDLastSave="1012" documentId="11_AD4D1D646341095ACB70008C251E688C5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FB8930B-C132-49E9-AD30-31AC345AC39D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Data" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="119">
   <si>
     <t>LP1</t>
   </si>
@@ -371,22 +371,13 @@
     <t>Nr Transformers</t>
   </si>
   <si>
-    <t>Nr Protection</t>
-  </si>
-  <si>
     <t>Fuse/breaker direction</t>
   </si>
   <si>
     <t>Disconnector direction</t>
   </si>
   <si>
-    <t>Breaker Type</t>
-  </si>
-  <si>
     <t>Transformer Type</t>
-  </si>
-  <si>
-    <t>Nr Breaker</t>
   </si>
   <si>
     <t>r</t>
@@ -933,15 +924,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4E8D12-5BBA-4420-83A4-3BE8673EEFAA}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>62</v>
       </c>
@@ -952,10 +943,10 @@
         <v>102</v>
       </c>
       <c r="E1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" t="s">
         <v>114</v>
-      </c>
-      <c r="F1" t="s">
-        <v>115</v>
       </c>
       <c r="G1" t="s">
         <v>111</v>
@@ -964,19 +955,10 @@
         <v>112</v>
       </c>
       <c r="I1" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K1" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1004,14 +986,8 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1039,14 +1015,8 @@
       <c r="I3" t="s">
         <v>91</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1074,14 +1044,8 @@
       <c r="I4" t="s">
         <v>91</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1109,14 +1073,8 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1144,14 +1102,8 @@
       <c r="I6" t="s">
         <v>91</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1179,14 +1131,8 @@
       <c r="I7" t="s">
         <v>91</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1214,14 +1160,8 @@
       <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1249,14 +1189,8 @@
       <c r="I9" t="s">
         <v>91</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1284,14 +1218,8 @@
       <c r="I10" t="s">
         <v>91</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1319,14 +1247,8 @@
       <c r="I11">
         <v>0</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1354,14 +1276,8 @@
       <c r="I12" t="s">
         <v>91</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1389,14 +1305,8 @@
       <c r="I13">
         <v>0</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1424,14 +1334,8 @@
       <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1459,14 +1363,8 @@
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1494,14 +1392,8 @@
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1529,14 +1421,8 @@
       <c r="I17">
         <v>0</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1564,14 +1450,8 @@
       <c r="I18" t="s">
         <v>91</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1599,14 +1479,8 @@
       <c r="I19">
         <v>0</v>
       </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1634,14 +1508,8 @@
       <c r="I20" t="s">
         <v>91</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1669,14 +1537,8 @@
       <c r="I21" t="s">
         <v>91</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1704,14 +1566,8 @@
       <c r="I22">
         <v>0</v>
       </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1739,14 +1595,8 @@
       <c r="I23" t="s">
         <v>91</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1774,14 +1624,8 @@
       <c r="I24" t="s">
         <v>91</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1809,14 +1653,8 @@
       <c r="I25">
         <v>0</v>
       </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1844,14 +1682,8 @@
       <c r="I26" t="s">
         <v>91</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1879,14 +1711,8 @@
       <c r="I27">
         <v>0</v>
       </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1914,14 +1740,8 @@
       <c r="I28" t="s">
         <v>91</v>
       </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -1949,14 +1769,8 @@
       <c r="I29" t="s">
         <v>91</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -1984,14 +1798,8 @@
       <c r="I30">
         <v>0</v>
       </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -2019,14 +1827,8 @@
       <c r="I31" t="s">
         <v>91</v>
       </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -2054,14 +1856,8 @@
       <c r="I32" t="s">
         <v>91</v>
       </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -2089,14 +1885,8 @@
       <c r="I33">
         <v>0</v>
       </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -2124,14 +1914,8 @@
       <c r="I34" t="s">
         <v>91</v>
       </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -2159,14 +1943,8 @@
       <c r="I35">
         <v>0</v>
       </c>
-      <c r="J35">
-        <v>1</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -2194,14 +1972,8 @@
       <c r="I36" t="s">
         <v>91</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -2229,14 +2001,8 @@
       <c r="I37" t="s">
         <v>91</v>
       </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -2262,12 +2028,6 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>2</v>
-      </c>
-      <c r="K38">
         <v>0</v>
       </c>
     </row>
@@ -2690,7 +2450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF1C9F0-4343-4AD1-924D-ED1403BEA6CF}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2698,13 +2458,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C1" t="s">
         <v>103</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E1" t="s">
         <v>107</v>
@@ -2827,7 +2587,7 @@
         <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
added load curve calculations
</commit_message>
<xml_diff>
--- a/BUS 2.xlsx
+++ b/BUS 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4264522ea65d2ce8/Dokumenter/NTNU/Master/Python Code/Git Repo/Simple-System-for-Power-System-Reliability-Calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1012" documentId="11_AD4D1D646341095ACB70008C251E688C5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FB8930B-C132-49E9-AD30-31AC345AC39D}"/>
+  <xr:revisionPtr revIDLastSave="1033" documentId="11_AD4D1D646341095ACB70008C251E688C5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04C61E2D-2A50-4903-8878-D2CA0E01D679}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Data" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Generation Data" sheetId="5" r:id="rId4"/>
     <sheet name="Backup Feeders" sheetId="6" r:id="rId5"/>
     <sheet name="Component Data" sheetId="4" r:id="rId6"/>
+    <sheet name="Weekly Load Factor" sheetId="7" r:id="rId7"/>
+    <sheet name="Daily Load Factor" sheetId="8" r:id="rId8"/>
+    <sheet name="Hourly Load Factor" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="129">
   <si>
     <t>LP1</t>
   </si>
@@ -387,6 +390,36 @@
   </si>
   <si>
     <t>AVG PEAK MW</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Load Factor</t>
+  </si>
+  <si>
+    <t>Day of week</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Winter Wkdy</t>
+  </si>
+  <si>
+    <t>Winter Wknd</t>
+  </si>
+  <si>
+    <t>Summer Wkdy</t>
+  </si>
+  <si>
+    <t>Summer Wknd</t>
+  </si>
+  <si>
+    <t>Spring/Fall Wkdy</t>
+  </si>
+  <si>
+    <t>Spring/Fall Wknd</t>
   </si>
 </sst>
 </file>
@@ -926,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4E8D12-5BBA-4420-83A4-3BE8673EEFAA}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -2750,4 +2783,1113 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84CC5F9A-BC37-4CDF-A03E-C2566F84A896}">
+  <dimension ref="A1:B53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>87.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>83.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>84.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>83.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>80.599999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>73.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>72.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>70.400000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>72.099999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>75.400000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>83.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>85.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>81.099999999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>88.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>89.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>86.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>81.599999999999994</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>80.099999999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>72.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>77.599999999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>72.900000000000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>72.599999999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>74.3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>74.400000000000006</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>88.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>90.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>94.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>95.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01B301D-9DAF-481A-8E17-9B76F3C525B9}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFA2D61-9FD1-40A3-B975-725D3E0EA1B3}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>67</v>
+      </c>
+      <c r="C2">
+        <v>78</v>
+      </c>
+      <c r="D2">
+        <v>64</v>
+      </c>
+      <c r="E2">
+        <v>74</v>
+      </c>
+      <c r="F2">
+        <v>63</v>
+      </c>
+      <c r="G2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>63</v>
+      </c>
+      <c r="C3">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <v>60</v>
+      </c>
+      <c r="E3">
+        <v>70</v>
+      </c>
+      <c r="F3">
+        <v>62</v>
+      </c>
+      <c r="G3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>68</v>
+      </c>
+      <c r="D4">
+        <v>58</v>
+      </c>
+      <c r="E4">
+        <v>66</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>59</v>
+      </c>
+      <c r="C5">
+        <v>66</v>
+      </c>
+      <c r="D5">
+        <v>56</v>
+      </c>
+      <c r="E5">
+        <v>65</v>
+      </c>
+      <c r="F5">
+        <v>58</v>
+      </c>
+      <c r="G5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>59</v>
+      </c>
+      <c r="C6">
+        <v>64</v>
+      </c>
+      <c r="D6">
+        <v>56</v>
+      </c>
+      <c r="E6">
+        <v>64</v>
+      </c>
+      <c r="F6">
+        <v>59</v>
+      </c>
+      <c r="G6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>58</v>
+      </c>
+      <c r="E7">
+        <v>62</v>
+      </c>
+      <c r="F7">
+        <v>65</v>
+      </c>
+      <c r="G7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>74</v>
+      </c>
+      <c r="C8">
+        <v>66</v>
+      </c>
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>62</v>
+      </c>
+      <c r="F8">
+        <v>72</v>
+      </c>
+      <c r="G8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>86</v>
+      </c>
+      <c r="C9">
+        <v>70</v>
+      </c>
+      <c r="D9">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>66</v>
+      </c>
+      <c r="F9">
+        <v>85</v>
+      </c>
+      <c r="G9">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>95</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
+      <c r="D10">
+        <v>87</v>
+      </c>
+      <c r="E10">
+        <v>81</v>
+      </c>
+      <c r="F10">
+        <v>95</v>
+      </c>
+      <c r="G10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>96</v>
+      </c>
+      <c r="C11">
+        <v>88</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <v>86</v>
+      </c>
+      <c r="F11">
+        <v>99</v>
+      </c>
+      <c r="G11">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>96</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>99</v>
+      </c>
+      <c r="E12">
+        <v>91</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>95</v>
+      </c>
+      <c r="C13">
+        <v>91</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <v>93</v>
+      </c>
+      <c r="F13">
+        <v>99</v>
+      </c>
+      <c r="G13">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>95</v>
+      </c>
+      <c r="C14">
+        <v>90</v>
+      </c>
+      <c r="D14">
+        <v>99</v>
+      </c>
+      <c r="E14">
+        <v>93</v>
+      </c>
+      <c r="F14">
+        <v>93</v>
+      </c>
+      <c r="G14">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>95</v>
+      </c>
+      <c r="C15">
+        <v>88</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>92</v>
+      </c>
+      <c r="F15">
+        <v>92</v>
+      </c>
+      <c r="G15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>93</v>
+      </c>
+      <c r="C16">
+        <v>87</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>91</v>
+      </c>
+      <c r="F16">
+        <v>90</v>
+      </c>
+      <c r="G16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>94</v>
+      </c>
+      <c r="C17">
+        <v>87</v>
+      </c>
+      <c r="D17">
+        <v>97</v>
+      </c>
+      <c r="E17">
+        <v>91</v>
+      </c>
+      <c r="F17">
+        <v>88</v>
+      </c>
+      <c r="G17">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>99</v>
+      </c>
+      <c r="C18">
+        <v>91</v>
+      </c>
+      <c r="D18">
+        <v>96</v>
+      </c>
+      <c r="E18">
+        <v>92</v>
+      </c>
+      <c r="F18">
+        <v>90</v>
+      </c>
+      <c r="G18">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+      <c r="D19">
+        <v>96</v>
+      </c>
+      <c r="E19">
+        <v>94</v>
+      </c>
+      <c r="F19">
+        <v>92</v>
+      </c>
+      <c r="G19">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>99</v>
+      </c>
+      <c r="D20">
+        <v>93</v>
+      </c>
+      <c r="E20">
+        <v>95</v>
+      </c>
+      <c r="F20">
+        <v>96</v>
+      </c>
+      <c r="G20">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>96</v>
+      </c>
+      <c r="C21">
+        <v>97</v>
+      </c>
+      <c r="D21">
+        <v>92</v>
+      </c>
+      <c r="E21">
+        <v>95</v>
+      </c>
+      <c r="F21">
+        <v>98</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>91</v>
+      </c>
+      <c r="C22">
+        <v>94</v>
+      </c>
+      <c r="D22">
+        <v>92</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>96</v>
+      </c>
+      <c r="G22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>83</v>
+      </c>
+      <c r="C23">
+        <v>92</v>
+      </c>
+      <c r="D23">
+        <v>93</v>
+      </c>
+      <c r="E23">
+        <v>93</v>
+      </c>
+      <c r="F23">
+        <v>90</v>
+      </c>
+      <c r="G23">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>73</v>
+      </c>
+      <c r="C24">
+        <v>87</v>
+      </c>
+      <c r="D24">
+        <v>87</v>
+      </c>
+      <c r="E24">
+        <v>88</v>
+      </c>
+      <c r="F24">
+        <v>80</v>
+      </c>
+      <c r="G24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>63</v>
+      </c>
+      <c r="C25">
+        <v>81</v>
+      </c>
+      <c r="D25">
+        <v>72</v>
+      </c>
+      <c r="E25">
+        <v>80</v>
+      </c>
+      <c r="F25">
+        <v>70</v>
+      </c>
+      <c r="G25">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added the option to use load curve and distributed generation curve, fixed some bugs
</commit_message>
<xml_diff>
--- a/BUS 2.xlsx
+++ b/BUS 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4264522ea65d2ce8/Dokumenter/NTNU/Master/Python Code/Git Repo/Simple-System-for-Power-System-Reliability-Calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1033" documentId="11_AD4D1D646341095ACB70008C251E688C5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04C61E2D-2A50-4903-8878-D2CA0E01D679}"/>
+  <xr:revisionPtr revIDLastSave="1047" documentId="11_AD4D1D646341095ACB70008C251E688C5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A694C0CD-96F0-40E2-81F2-BF0E71F74501}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Data" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="130">
   <si>
     <t>LP1</t>
   </si>
@@ -347,9 +347,6 @@
     <t>Lim MVAR</t>
   </si>
   <si>
-    <t>inf</t>
-  </si>
-  <si>
     <t>BS1</t>
   </si>
   <si>
@@ -386,12 +383,6 @@
     <t>r</t>
   </si>
   <si>
-    <t>AVG E cap</t>
-  </si>
-  <si>
-    <t>AVG PEAK MW</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
@@ -420,6 +411,18 @@
   </si>
   <si>
     <t>Spring/Fall Wknd</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Lim MW</t>
+  </si>
+  <si>
+    <t>E cap</t>
+  </si>
+  <si>
+    <t>Inf</t>
   </si>
 </sst>
 </file>
@@ -976,19 +979,19 @@
         <v>102</v>
       </c>
       <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
         <v>113</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
         <v>114</v>
-      </c>
-      <c r="G1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2076,7 +2079,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2481,26 +2484,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF1C9F0-4343-4AD1-924D-ED1403BEA6CF}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C1" t="s">
         <v>103</v>
       </c>
       <c r="D1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2508,38 +2511,49 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>67</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>69</v>
       </c>
-      <c r="B4">
+      <c r="B10">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>104</v>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2559,10 +2573,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
         <v>109</v>
-      </c>
-      <c r="C1" t="s">
-        <v>110</v>
       </c>
       <c r="D1" t="s">
         <v>80</v>
@@ -2570,7 +2584,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
         <v>68</v>
@@ -2584,7 +2598,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
         <v>74</v>
@@ -2620,7 +2634,7 @@
         <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D1" t="s">
         <v>80</v>
@@ -2790,17 +2804,17 @@
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection sqref="A1:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3229,17 +3243,17 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3308,32 +3322,32 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
         <v>122</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>123</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>124</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>125</v>
-      </c>
-      <c r="E1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>